<commit_message>
Se han aplicado correciones adicionales aldocumento de avances
</commit_message>
<xml_diff>
--- a/Analisis/ReporteAvances/Reporte_1/Graficas/GraficaRecoleecion.xlsx
+++ b/Analisis/ReporteAvances/Reporte_1/Graficas/GraficaRecoleecion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Andrew/Documents/ESCOM/TT2/TT2/Desarrollo/Clasificador/Resultados/Prueba.08.10.2019/Reporte/Graficas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Andrew/Documents/ESCOM/TT2/TT2/Analisis/ReporteAvances/Reporte_1/Graficas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A480D29-306F-404E-9D90-2A4ED4EA176A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111BAA03-4D69-7C4B-BA6C-238C86727C2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28800" windowHeight="16600" activeTab="1" xr2:uid="{A6691E8A-B295-AE49-AFAE-55920EB11DBC}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16600" activeTab="1" xr2:uid="{A6691E8A-B295-AE49-AFAE-55920EB11DBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Recoleción" sheetId="1" r:id="rId1"/>
@@ -726,7 +726,7 @@
                   <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>653</c:v>
+                  <c:v>647</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2633,7 +2633,7 @@
   <dimension ref="A3:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2686,7 +2686,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>653</v>
+        <v>647</v>
       </c>
     </row>
   </sheetData>

</xml_diff>